<commit_message>
Refactor button labels and add new button for "المدائح والتماجيد" and edited the ppt files
</commit_message>
<xml_diff>
--- a/بيانات القداسات.xlsx
+++ b/بيانات القداسات.xlsx
@@ -10435,7 +10435,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11630,6 +11630,48 @@
       </c>
       <c r="E56" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>انظروا يديه تأملوا رجليه</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>{E1A31474-7F00-4B7D-90FD-A67415E32872}</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1582</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1596</v>
+      </c>
+      <c r="E57" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>يا ربنا مولى السلام</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>{325B4DE6-FA63-4B6D-827F-BCC78EF1FEC9}</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1597</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1639</v>
+      </c>
+      <c r="E58" t="n">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -24094,7 +24136,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24580,12 +24622,12 @@
     <row r="23" ht="18.75" customHeight="1">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ابصالية آدام لعيد التجلي</t>
+          <t>ابصالية آدام للخمسين</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{EF0F739B-A8DE-419D-8D45-757AA9347AB5}</t>
+          <t>{43AC03AD-AC75-480D-987F-66CB8CBE3883}</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -24601,12 +24643,12 @@
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ابصالية واطس لعيد التجلي</t>
+          <t>ابصالية آدام لعيد التجلي</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{95F02DE0-6540-4250-B6D4-213F4C9B73FC}</t>
+          <t>{EF0F739B-A8DE-419D-8D45-757AA9347AB5}</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -24622,54 +24664,54 @@
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ابصالية آدام لصوم العذراء</t>
+          <t>ابصالية واطس لعيد التجلي</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{2908EF39-9CFE-4101-AED3-B54AD30D5A78}</t>
+          <t>{95F02DE0-6540-4250-B6D4-213F4C9B73FC}</t>
         </is>
       </c>
       <c r="C25" t="n">
         <v>544</v>
       </c>
       <c r="D25" t="n">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="E25" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ابصالية واطس لصوم العذراء</t>
+          <t>ابصالية آدام لصوم العذراء</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{222D1CFF-8162-4F43-A7FC-D6E04CE630E4}</t>
+          <t>{2908EF39-9CFE-4101-AED3-B54AD30D5A78}</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="D26" t="n">
         <v>598</v>
       </c>
       <c r="E26" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ابصالية آدام لعيد العذراء</t>
+          <t>ابصالية واطس لصوم العذراء</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>{CF62ACEE-48F9-4ABA-ADDC-6180BEC4873D}</t>
+          <t>{222D1CFF-8162-4F43-A7FC-D6E04CE630E4}</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -24685,691 +24727,691 @@
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ابصالية واطس لعيد العذراء</t>
+          <t>ابصالية آدام لعيد العذراء</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{E2D40FD7-171F-428B-86DB-65B332AB25F3}</t>
+          <t>{CF62ACEE-48F9-4ABA-ADDC-6180BEC4873D}</t>
         </is>
       </c>
       <c r="C28" t="n">
         <v>623</v>
       </c>
       <c r="D28" t="n">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E28" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" ht="18.75" customHeight="1">
       <c r="A29" t="inlineStr">
         <is>
-          <t>تسبحة الأيام</t>
+          <t>ابصالية واطس لعيد العذراء</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{34B2EF10-1881-4BA7-95A7-7AB2F6F6651C}</t>
+          <t>{E2D40FD7-171F-428B-86DB-65B332AB25F3}</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D29" t="n">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ابصالية الأحد 1</t>
+          <t>تسبحة الأيام</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{F8548FDB-8D40-484A-8D19-36EC50E838FD}</t>
+          <t>{34B2EF10-1881-4BA7-95A7-7AB2F6F6651C}</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>651</v>
+        <v>674</v>
       </c>
       <c r="D30" t="n">
         <v>674</v>
       </c>
       <c r="E30" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" ht="18.75" customHeight="1">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ابصالية الأحد الثانية</t>
+          <t>ابصالية الأحد 1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{F263153B-C7A8-4E6B-AACA-6F05AF050F2E}</t>
+          <t>{F8548FDB-8D40-484A-8D19-36EC50E838FD}</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>675</v>
       </c>
       <c r="D31" t="n">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="E31" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ابصالية الاثنين</t>
+          <t>ابصالية الأحد الثانية</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>{C966C7AC-73F9-4177-AA7F-71D0428224AF}</t>
+          <t>{F263153B-C7A8-4E6B-AACA-6F05AF050F2E}</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="D32" t="n">
-        <v>737</v>
+        <v>730</v>
       </c>
       <c r="E32" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ابصالية الثلاثاء</t>
+          <t>ابصالية الاثنين</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{31645468-E515-4F5A-85DB-DEE662F6432A}</t>
+          <t>{C966C7AC-73F9-4177-AA7F-71D0428224AF}</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="D33" t="n">
-        <v>749</v>
+        <v>761</v>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" ht="18.75" customHeight="1">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ابصالية الأربعاء</t>
+          <t>ابصالية الثلاثاء</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{8ABA75EA-D793-46A0-8AE2-5B61A6B4FD7E}</t>
+          <t>{31645468-E515-4F5A-85DB-DEE662F6432A}</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>750</v>
+        <v>762</v>
       </c>
       <c r="D34" t="n">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E34" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ابصالية الخميس</t>
+          <t>ابصالية الأربعاء</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>{02352F94-02C4-4D7F-9247-697DA282E7C9}</t>
+          <t>{8ABA75EA-D793-46A0-8AE2-5B61A6B4FD7E}</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D35" t="n">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="E35" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" ht="18.75" customHeight="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ابصالية الجمعة</t>
+          <t>ابصالية الخميس</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{E8504067-DC7B-4818-8157-B947A0A74D9A}</t>
+          <t>{02352F94-02C4-4D7F-9247-697DA282E7C9}</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="D36" t="n">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="E36" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ابصالية السبت</t>
+          <t>ابصالية الجمعة</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{BF504610-6275-426C-A939-798A885C5C71}</t>
+          <t>{E8504067-DC7B-4818-8157-B947A0A74D9A}</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="D37" t="n">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="E37" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>مقدمة الثيؤطوكيات الأدام</t>
+          <t>ابصالية السبت</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>{E358EDB7-F8FF-43DA-A8B6-81839E23E4C6}</t>
+          <t>{BF504610-6275-426C-A939-798A885C5C71}</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="D38" t="n">
-        <v>852</v>
+        <v>871</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" ht="18.75" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>مقدمة الثيؤطوكيات الواطس</t>
+          <t>مقدمة الثيؤطوكيات الأدام</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>{F96B080A-3FB2-430B-9BED-E692E913A9B0}</t>
+          <t>{E358EDB7-F8FF-43DA-A8B6-81839E23E4C6}</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>853</v>
+        <v>872</v>
       </c>
       <c r="D39" t="n">
-        <v>854</v>
+        <v>876</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" ht="18.75" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأحد 1-6</t>
+          <t>مقدمة الثيؤطوكيات الواطس</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{8B50A9B8-162A-45FD-A40D-5405E501F1E6}</t>
+          <t>{F96B080A-3FB2-430B-9BED-E692E913A9B0}</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>855</v>
+        <v>877</v>
       </c>
       <c r="D40" t="n">
-        <v>939</v>
+        <v>878</v>
       </c>
       <c r="E40" t="n">
-        <v>85</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأحد 7-9</t>
+          <t>ثيؤطوكية الأحد 1-6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>{64CE0420-479F-4F12-AE0C-F1218BF21635}</t>
+          <t>{8B50A9B8-162A-45FD-A40D-5405E501F1E6}</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>940</v>
+        <v>879</v>
       </c>
       <c r="D41" t="n">
-        <v>991</v>
+        <v>963</v>
       </c>
       <c r="E41" t="n">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" ht="18.75" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأحد 10</t>
+          <t>ثيؤطوكية الأحد 7-9</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>{797B381C-F875-4BB4-8ACB-A5852FFBD8FC}</t>
+          <t>{64CE0420-479F-4F12-AE0C-F1218BF21635}</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>992</v>
+        <v>964</v>
       </c>
       <c r="D42" t="n">
-        <v>997</v>
+        <v>1015</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" ht="18.75" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأحد 11-15</t>
+          <t>ثيؤطوكية الأحد 10</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{67866127-A8D5-451C-B0C2-1CE6E6FBCD1F}</t>
+          <t>{797B381C-F875-4BB4-8ACB-A5852FFBD8FC}</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>998</v>
+        <v>1016</v>
       </c>
       <c r="D43" t="n">
-        <v>1046</v>
+        <v>1021</v>
       </c>
       <c r="E43" t="n">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الإثنين</t>
+          <t>ثيؤطوكية الأحد 11-15</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{5022D768-2E12-4BEA-8D76-E3896BD58932}</t>
+          <t>{67866127-A8D5-451C-B0C2-1CE6E6FBCD1F}</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1047</v>
+        <v>1022</v>
       </c>
       <c r="D44" t="n">
-        <v>1091</v>
+        <v>1070</v>
       </c>
       <c r="E44" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الثلاثاء</t>
+          <t>ثيؤطوكية الإثنين</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{D1BFEE47-99F3-4046-8C36-B6397205435B}</t>
+          <t>{5022D768-2E12-4BEA-8D76-E3896BD58932}</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1092</v>
+        <v>1071</v>
       </c>
       <c r="D45" t="n">
-        <v>1139</v>
+        <v>1115</v>
       </c>
       <c r="E45" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" ht="18.75" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأربعاء</t>
+          <t>ثيؤطوكية الثلاثاء</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{5AD56D85-2906-43FB-98E9-FB96F1B37293}</t>
+          <t>{D1BFEE47-99F3-4046-8C36-B6397205435B}</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1140</v>
+        <v>1116</v>
       </c>
       <c r="D46" t="n">
-        <v>1184</v>
+        <v>1163</v>
       </c>
       <c r="E46" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الخميس</t>
+          <t>ثيؤطوكية الأربعاء</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{88249BFF-471A-47A1-B7BC-E5A5093EC8D7}</t>
+          <t>{5AD56D85-2906-43FB-98E9-FB96F1B37293}</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1185</v>
+        <v>1164</v>
       </c>
       <c r="D47" t="n">
-        <v>1280</v>
+        <v>1208</v>
       </c>
       <c r="E47" t="n">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الجمعة</t>
+          <t>ثيؤطوكية الخميس</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{6C9361D4-74F3-4201-B28D-7EB59C9D9A46}</t>
+          <t>{88249BFF-471A-47A1-B7BC-E5A5093EC8D7}</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1281</v>
+        <v>1209</v>
       </c>
       <c r="D48" t="n">
-        <v>1309</v>
+        <v>1304</v>
       </c>
       <c r="E48" t="n">
-        <v>29</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" ht="18.75" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ثيؤطوكية السبت</t>
+          <t>ثيؤطوكية الجمعة</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{25CBC7C4-A68C-4EBD-B127-98DA707B3413}</t>
+          <t>{6C9361D4-74F3-4201-B28D-7EB59C9D9A46}</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1310</v>
+        <v>1305</v>
       </c>
       <c r="D49" t="n">
-        <v>1346</v>
+        <v>1333</v>
       </c>
       <c r="E49" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ثيؤطوكية الأحد 16-18</t>
+          <t>ثيؤطوكية السبت</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{4E843BF3-1D30-4BED-905C-E66AA3D90EC5}</t>
+          <t>{25CBC7C4-A68C-4EBD-B127-98DA707B3413}</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1347</v>
+        <v>1334</v>
       </c>
       <c r="D50" t="n">
-        <v>1359</v>
+        <v>1370</v>
       </c>
       <c r="E50" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" ht="18.75" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>لبش الإثنين</t>
+          <t>ثيؤطوكية الأحد 16-18</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{B08DAA27-DC93-470F-8EE4-DBA2CDED73FF}</t>
+          <t>{4E843BF3-1D30-4BED-905C-E66AA3D90EC5}</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1360</v>
+        <v>1371</v>
       </c>
       <c r="D51" t="n">
-        <v>1371</v>
+        <v>1383</v>
       </c>
       <c r="E51" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" ht="18.75" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>لبش الثلاثاء</t>
+          <t>لبش الإثنين</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>{EA64C1D5-8011-4ED1-AECA-ACA0D1D96925}</t>
+          <t>{B08DAA27-DC93-470F-8EE4-DBA2CDED73FF}</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1372</v>
+        <v>1384</v>
       </c>
       <c r="D52" t="n">
-        <v>1380</v>
+        <v>1395</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" ht="18.75" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>لبش الأربعاء</t>
+          <t>لبش الثلاثاء</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>{824D594F-C079-4552-882A-CC297F319D7D}</t>
+          <t>{EA64C1D5-8011-4ED1-AECA-ACA0D1D96925}</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1381</v>
+        <v>1396</v>
       </c>
       <c r="D53" t="n">
-        <v>1395</v>
+        <v>1404</v>
       </c>
       <c r="E53" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
       <c r="A54" t="inlineStr">
         <is>
-          <t>لبش الخميس</t>
+          <t>لبش الأربعاء</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>{260E1FAC-A9F6-4E94-BAAB-EFD045CD242D}</t>
+          <t>{824D594F-C079-4552-882A-CC297F319D7D}</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1396</v>
+        <v>1405</v>
       </c>
       <c r="D54" t="n">
-        <v>1412</v>
+        <v>1419</v>
       </c>
       <c r="E54" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" ht="18.75" customHeight="1">
       <c r="A55" t="inlineStr">
         <is>
-          <t>لبش الجمعة</t>
+          <t>لبش الخميس</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>{27A6E4EC-9C9A-4029-8EAF-A984FA647997}</t>
+          <t>{260E1FAC-A9F6-4E94-BAAB-EFD045CD242D}</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1413</v>
+        <v>1420</v>
       </c>
       <c r="D55" t="n">
-        <v>1432</v>
+        <v>1436</v>
       </c>
       <c r="E55" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" ht="18.75" customHeight="1">
       <c r="A56" t="inlineStr">
         <is>
-          <t>شيرات السبت 1</t>
+          <t>لبش الجمعة</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>{FA5AF629-FC64-4123-92EA-193DFE2229CC}</t>
+          <t>{27A6E4EC-9C9A-4029-8EAF-A984FA647997}</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1433</v>
+        <v>1437</v>
       </c>
       <c r="D56" t="n">
-        <v>1444</v>
+        <v>1456</v>
       </c>
       <c r="E56" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" ht="18.75" customHeight="1">
       <c r="A57" t="inlineStr">
         <is>
-          <t>شيرات السبت 2</t>
+          <t>شيرات السبت 1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>{2DF7B6FE-B056-4813-B72C-DFE470371815}</t>
+          <t>{FA5AF629-FC64-4123-92EA-193DFE2229CC}</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1445</v>
+        <v>1457</v>
       </c>
       <c r="D57" t="n">
-        <v>1460</v>
+        <v>1468</v>
       </c>
       <c r="E57" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" ht="18.75" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>مقدمة الدفنار</t>
+          <t>شيرات السبت 2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>{DBBEB49F-3396-41D0-81FF-0A028C3CB4DA}</t>
+          <t>{2DF7B6FE-B056-4813-B72C-DFE470371815}</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1461</v>
+        <v>1469</v>
       </c>
       <c r="D58" t="n">
-        <v>1461</v>
+        <v>1484</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" ht="18.75" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>مقدمة الدفنار الآدام</t>
+          <t>مقدمة الدفنار</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>{0420AA0C-B21A-478D-88EA-8378E9539EDE}</t>
+          <t>{DBBEB49F-3396-41D0-81FF-0A028C3CB4DA}</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1462</v>
+        <v>1485</v>
       </c>
       <c r="D59" t="n">
-        <v>1465</v>
+        <v>1485</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" ht="18.75" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
-          <t>مقدمة الدفنار الواطس</t>
+          <t>مقدمة الدفنار الآدام</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>{F2541D73-C210-4196-BE50-DF6E6142A86C}</t>
+          <t>{0420AA0C-B21A-478D-88EA-8378E9539EDE}</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1466</v>
+        <v>1486</v>
       </c>
       <c r="D60" t="n">
-        <v>1469</v>
+        <v>1489</v>
       </c>
       <c r="E60" t="n">
         <v>4</v>
@@ -25378,103 +25420,103 @@
     <row r="61" ht="18.75" customHeight="1">
       <c r="A61" t="inlineStr">
         <is>
-          <t>الدفنار</t>
+          <t>مقدمة الدفنار الواطس</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>{A509B738-02BB-455A-944E-9E56D85C8942}</t>
+          <t>{F2541D73-C210-4196-BE50-DF6E6142A86C}</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1470</v>
+        <v>1490</v>
       </c>
       <c r="D61" t="n">
-        <v>1471</v>
+        <v>1493</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" ht="18.75" customHeight="1">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ختام الثؤطوكيات الادام</t>
+          <t>الدفنار</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>{14A3A43C-A9F7-45A8-A510-EE3F33D99572}</t>
+          <t>{A509B738-02BB-455A-944E-9E56D85C8942}</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1472</v>
+        <v>1494</v>
       </c>
       <c r="D62" t="n">
-        <v>1488</v>
+        <v>1495</v>
       </c>
       <c r="E62" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" ht="18.75" customHeight="1">
       <c r="A63" t="inlineStr">
         <is>
-          <t>ختام الثيؤطوكيات الواطس</t>
+          <t>ختام الثؤطوكيات الادام</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>{BF439D71-64D1-4376-8E4A-812437425EBB}</t>
+          <t>{14A3A43C-A9F7-45A8-A510-EE3F33D99572}</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1489</v>
+        <v>1496</v>
       </c>
       <c r="D63" t="n">
-        <v>1508</v>
+        <v>1512</v>
       </c>
       <c r="E63" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" ht="18.75" customHeight="1">
       <c r="A64" t="inlineStr">
         <is>
-          <t>قانون الايمان</t>
+          <t>ختام الثيؤطوكيات الواطس</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>{A12368B5-4E89-4682-AF79-DC1979BA120B}</t>
+          <t>{BF439D71-64D1-4376-8E4A-812437425EBB}</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1509</v>
+        <v>1513</v>
       </c>
       <c r="D64" t="n">
-        <v>1523</v>
+        <v>1532</v>
       </c>
       <c r="E64" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" ht="18.75" customHeight="1">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ختام التسبحة</t>
+          <t>قانون الايمان</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>{BABBF91F-DC4B-4DBC-A6C1-054AEA7290F3}</t>
+          <t>{A12368B5-4E89-4682-AF79-DC1979BA120B}</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1524</v>
+        <v>1533</v>
       </c>
       <c r="D65" t="n">
-        <v>1538</v>
+        <v>1547</v>
       </c>
       <c r="E65" t="n">
         <v>15</v>
@@ -25483,21 +25525,42 @@
     <row r="66" ht="18.75" customHeight="1">
       <c r="A66" t="inlineStr">
         <is>
+          <t>ختام التسبحة</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>{BABBF91F-DC4B-4DBC-A6C1-054AEA7290F3}</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1548</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1562</v>
+      </c>
+      <c r="E66" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>قدوس قدوس قدوس</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>{F2F363F3-5DD8-474B-94A0-6895758AB76D}</t>
         </is>
       </c>
-      <c r="C66" t="n">
-        <v>1539</v>
-      </c>
-      <c r="D66" t="n">
-        <v>1543</v>
-      </c>
-      <c r="E66" t="n">
+      <c r="C67" t="n">
+        <v>1563</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1567</v>
+      </c>
+      <c r="E67" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
aashyaSnawy finished, global load_background and relative path, resolved errors
</commit_message>
<xml_diff>
--- a/بيانات القداسات.xlsx
+++ b/بيانات القداسات.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="القداس" sheetId="1" state="visible" r:id="rId1"/>
@@ -76,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -93,14 +93,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -472,7 +469,7 @@
   </sheetPr>
   <dimension ref="A1:E473"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -480,9 +477,9 @@
   <cols>
     <col width="59.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="42.86214285714286" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -4250,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" ht="18.75" customHeight="1">
+    <row r="180" ht="19.5" customHeight="1">
       <c r="A180" t="inlineStr">
         <is>
           <t>مرد مزمور عرس قانا الجليل</t>
@@ -4271,7 +4268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" ht="18.75" customHeight="1">
+    <row r="181" ht="19.5" customHeight="1">
       <c r="A181" t="inlineStr">
         <is>
           <t>مرد مزمور دخول المسيح الهيكل</t>
@@ -4292,7 +4289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" ht="18.75" customHeight="1">
+    <row r="182" ht="19.5" customHeight="1">
       <c r="A182" t="inlineStr">
         <is>
           <t>مرد مزمور البشارة</t>
@@ -4313,7 +4310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" ht="18.75" customHeight="1">
+    <row r="183" ht="19.5" customHeight="1">
       <c r="A183" t="inlineStr">
         <is>
           <t>مرد مزمور الشعانين</t>
@@ -4334,7 +4331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" ht="18.75" customHeight="1">
+    <row r="184" ht="19.5" customHeight="1">
       <c r="A184" t="inlineStr">
         <is>
           <t>مرد المزمور القيامة</t>
@@ -4355,7 +4352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" ht="18.75" customHeight="1">
+    <row r="185" ht="19.5" customHeight="1">
       <c r="A185" t="inlineStr">
         <is>
           <t>مرد مزمور الصعود</t>
@@ -4376,7 +4373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" ht="18.75" customHeight="1">
+    <row r="186" ht="19.5" customHeight="1">
       <c r="A186" t="inlineStr">
         <is>
           <t>مرد مزمور العنصرة</t>
@@ -4397,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" ht="18.75" customHeight="1">
+    <row r="187" ht="19.5" customHeight="1">
       <c r="A187" t="inlineStr">
         <is>
           <t>مرد مزمور التجلي</t>
@@ -4418,7 +4415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" ht="18.75" customHeight="1">
+    <row r="188" ht="19.5" customHeight="1">
       <c r="A188" t="inlineStr">
         <is>
           <t>مرد مزمور ال29 من الشهر</t>
@@ -4439,7 +4436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" ht="18.75" customHeight="1">
+    <row r="189" ht="19.5" customHeight="1">
       <c r="A189" t="inlineStr">
         <is>
           <t>مرد المزمور</t>
@@ -4460,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" ht="18.75" customHeight="1">
+    <row r="190" ht="19.5" customHeight="1">
       <c r="A190" t="inlineStr">
         <is>
           <t>مقدمة الانجيل</t>
@@ -4481,7 +4478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" ht="18.75" customHeight="1">
+    <row r="191" ht="19.5" customHeight="1">
       <c r="A191" t="inlineStr">
         <is>
           <t>الانجيل قبطي</t>
@@ -4502,7 +4499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" ht="18.75" customHeight="1">
+    <row r="192" ht="19.5" customHeight="1">
       <c r="A192" t="inlineStr">
         <is>
           <t>المزمور</t>
@@ -4523,7 +4520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" ht="18.75" customHeight="1">
+    <row r="193" ht="19.5" customHeight="1">
       <c r="A193" t="inlineStr">
         <is>
           <t>فليرفعوه</t>
@@ -4544,7 +4541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" ht="18.75" customHeight="1">
+    <row r="194" ht="19.5" customHeight="1">
       <c r="A194" t="inlineStr">
         <is>
           <t>الانجيل</t>
@@ -4565,7 +4562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" ht="18.75" customHeight="1">
+    <row r="195" ht="19.5" customHeight="1">
       <c r="A195" t="inlineStr">
         <is>
           <t>مرد انجيل النيروز</t>
@@ -10445,9 +10442,9 @@
   <cols>
     <col width="41.005" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -11632,7 +11629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="18.75" customHeight="1">
       <c r="A57" t="inlineStr">
         <is>
           <t>انظروا يديه تأملوا رجليه</t>
@@ -11653,7 +11650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="18.75" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
           <t>يا ربنا مولى السلام</t>
@@ -11695,9 +11692,9 @@
   <cols>
     <col width="20.29071428571428" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -12049,9 +12046,9 @@
   <cols>
     <col width="15.29071428571429" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -12445,9 +12442,9 @@
   <cols>
     <col width="17.005" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -13114,9 +13111,9 @@
   <cols>
     <col width="28.43357142857143" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -18543,9 +18540,9 @@
   <cols>
     <col width="20.71928571428571" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -19500,9 +19497,9 @@
   <cols>
     <col width="19.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -21203,9 +21200,9 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -21213,9 +21210,9 @@
   <cols>
     <col width="30.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -21274,1169 +21271,1169 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{03B57C83-EC25-40DE-9969-D1416437B668}</t>
+          <t>{40B60A3B-1E1C-423C-A2AC-B3081CEEE693}</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E3" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
-          <t>صلاة الشكر 2</t>
+          <t>طوبه هينا الصغيرة</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{AC3A87BC-30B2-45B8-8A57-8667467EF7D6}</t>
+          <t>{8FB4FAC1-B1DC-4F98-8E39-10134B6B80AB}</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ارباع الناقوس</t>
+          <t>تكملة في حضور الاسقف</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{8B27D80D-B166-4555-85E2-39A92ED59D83}</t>
+          <t>{F76B0D75-0474-45B5-B79F-7416F354543A}</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D5" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ارباع الناقوس الادام</t>
+          <t>طوبه هينا الكبيرة</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{D02C088A-01E0-4A8C-8D73-21E3FD3616EB}</t>
+          <t>{8DD21CDE-CB6B-4D5B-B995-D2747AB69ED1}</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D6" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>أرباع الناقوس الواطس</t>
+          <t>تكملة طوبه هينا الكبيرة</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{9495E38B-CE03-4E75-AED4-960DE95BA747}</t>
+          <t>{E5147E52-9DB8-46B0-B31A-60CAADE66604}</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>تكملة ارباع الناقوس</t>
+          <t>تكملة صلاة الشكر</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{0120814B-6347-4FF3-9CA8-883FC9FEF728}</t>
+          <t>{02B17B5A-01EB-411F-9680-31ECEA7A4AA6}</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D8" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
-          <t>تكملة ارباع الناقوس 2</t>
+          <t>ارباع الناقوس</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{3C444163-4B5E-4306-8A8A-489D9AF24A2A}</t>
+          <t>{8B27D80D-B166-4555-85E2-39A92ED59D83}</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ختام ارباع الناقوس</t>
+          <t>ارباع الناقوس الادام</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{52EB6B04-BCFD-460D-A692-2D541D7484D5}</t>
+          <t>{D02C088A-01E0-4A8C-8D73-21E3FD3616EB}</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D10" t="n">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" ht="18.75" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ختام ارباع الناقوس الفرايحي</t>
+          <t>أرباع الناقوس الواطس</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{B87EBA1A-E0E4-4E68-87D7-3C4A798CF278}</t>
+          <t>{9495E38B-CE03-4E75-AED4-960DE95BA747}</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" ht="18.75" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>اوشية الراقدين</t>
+          <t>تكملة ارباع الناقوس</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{83E6BC33-A9EC-45CA-89B6-24EFBC51B654}</t>
+          <t>{0120814B-6347-4FF3-9CA8-883FC9FEF728}</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="D12" t="n">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="E12" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" ht="18.75" customHeight="1">
       <c r="A13" t="inlineStr">
         <is>
-          <t>تفضل يا رب</t>
+          <t>ربع بطرس و بولس</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{D8AFA182-3999-4072-94E9-F65D50B876B9}</t>
+          <t>{3C444163-4B5E-4306-8A8A-489D9AF24A2A}</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="D13" t="n">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="E13" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="18.75" customHeight="1">
       <c r="A14" t="inlineStr">
         <is>
-          <t>اوشية المرضي</t>
+          <t>ربع مارمرقس</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{069F7A79-999B-4223-82AE-CAF356118167}</t>
+          <t>{3CEEB174-A27F-4ACB-B72B-4D39D2FC700F}</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>179</v>
+        <v>87</v>
       </c>
       <c r="D14" t="n">
-        <v>213</v>
+        <v>88</v>
       </c>
       <c r="E14" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" ht="18.75" customHeight="1">
       <c r="A15" t="inlineStr">
         <is>
-          <t>السبع طرايق</t>
+          <t>ربع اسطفانوس</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{385BAEA4-D798-4AD0-920D-ADEC0B972186}</t>
+          <t>{A7614D8D-F4B4-41D2-A880-10234332DD2F}</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>214</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>344</v>
+        <v>89</v>
       </c>
       <c r="E15" t="n">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" ht="18.75" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
-          <t>اوشية المسافرين</t>
+          <t>ربع مارجرجس</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{A059EEC9-5D25-453F-A956-A2E149F0773C}</t>
+          <t>{4E9FE7F7-74A7-4CEE-8CA7-DD64178EF766}</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>345</v>
+        <v>90</v>
       </c>
       <c r="D16" t="n">
-        <v>372</v>
+        <v>91</v>
       </c>
       <c r="E16" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" ht="18.75" customHeight="1">
       <c r="A17" t="inlineStr">
         <is>
-          <t>اوشية القرابين</t>
+          <t>ربع مارمينا</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{2C897F14-44CC-430E-9BE1-EB379FE7A9C7}</t>
+          <t>{6961CDD1-5D71-496E-B14F-1243FFFD6BBB}</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>373</v>
+        <v>92</v>
       </c>
       <c r="D17" t="n">
-        <v>401</v>
+        <v>93</v>
       </c>
       <c r="E17" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" t="inlineStr">
         <is>
-          <t>فلنسبح مع الملائكة</t>
+          <t>ربع فيلوباتير ميرقوريوس</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{2ECE1F1B-C143-4CE2-B550-348BEE185974}</t>
+          <t>{7666EA7B-1BFC-44EC-AB49-26F16C714438}</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>402</v>
+        <v>94</v>
       </c>
       <c r="D18" t="n">
-        <v>418</v>
+        <v>95</v>
       </c>
       <c r="E18" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" t="inlineStr">
         <is>
-          <t>مقدمة الذوكصولوجيات</t>
+          <t>ختام ارباع الناقوس</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{D72E4090-F25E-47FA-91CC-49FA1BFA5556}</t>
+          <t>{52EB6B04-BCFD-460D-A692-2D541D7484D5}</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>419</v>
+        <v>96</v>
       </c>
       <c r="D19" t="n">
-        <v>431</v>
+        <v>100</v>
       </c>
       <c r="E19" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
       <c r="A20" t="inlineStr">
         <is>
-          <t>الذكصولوجيات</t>
+          <t>ختام ارباع الناقوس الفرايحي</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{A5B9CE2F-90E3-44D7-B22F-CAE6783C8E2F}</t>
+          <t>{B87EBA1A-E0E4-4E68-87D7-3C4A798CF278}</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>432</v>
+        <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>432</v>
+        <v>111</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="1">
       <c r="A21" t="inlineStr">
         <is>
-          <t>قانون الإيمان</t>
+          <t>اوشية الراقدين</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{BA246F91-8526-4A8F-8E43-CEF5EEE442BB}</t>
+          <t>{83E6BC33-A9EC-45CA-89B6-24EFBC51B654}</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>433</v>
+        <v>112</v>
       </c>
       <c r="D21" t="n">
-        <v>451</v>
+        <v>163</v>
       </c>
       <c r="E21" t="n">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" ht="18.75" customHeight="1">
       <c r="A22" t="inlineStr">
         <is>
-          <t>افنوتي ناي نان</t>
+          <t>تفضل يا رب</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{61880C5D-7B19-4DA9-9517-587F0006E7A4}</t>
+          <t>{D8AFA182-3999-4072-94E9-F65D50B876B9}</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>452</v>
+        <v>164</v>
       </c>
       <c r="D22" t="n">
-        <v>460</v>
+        <v>189</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ايطاف اني اسخاي</t>
+          <t>اوشية المرضي</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{60A6EF5E-A7D1-4E39-AAE6-A0EA92726711}</t>
+          <t>{069F7A79-999B-4223-82AE-CAF356118167}</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>461</v>
+        <v>190</v>
       </c>
       <c r="D23" t="n">
-        <v>474</v>
+        <v>224</v>
       </c>
       <c r="E23" t="n">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" t="inlineStr">
         <is>
-          <t>طرح عيد الصليب</t>
+          <t>السبع طرايق</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{17F6A454-5ABF-4DFB-A78A-D146D086082D}</t>
+          <t>{385BAEA4-D798-4AD0-920D-ADEC0B972186}</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>475</v>
+        <v>225</v>
       </c>
       <c r="D24" t="n">
-        <v>479</v>
+        <v>355</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" t="inlineStr">
         <is>
-          <t>طرح اخر لعيد الصليب</t>
+          <t>اوشية المسافرين</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{0BD005D7-2E83-417A-9686-5430EAAF391B}</t>
+          <t>{A059EEC9-5D25-453F-A956-A2E149F0773C}</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>480</v>
+        <v>356</v>
       </c>
       <c r="D25" t="n">
-        <v>484</v>
+        <v>383</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>مرد طرح عيد الصليب</t>
+          <t>اوشية القرابين</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{68F134B0-811C-48F0-A7D0-5BB19CE61443}</t>
+          <t>{2C897F14-44CC-430E-9BE1-EB379FE7A9C7}</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>485</v>
+        <v>384</v>
       </c>
       <c r="D26" t="n">
-        <v>485</v>
+        <v>412</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>أفرحى يا مريم</t>
+          <t>فلنسبح مع الملائكة</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>{1C20AEEF-0DEB-4F74-A46A-AFC5A06DC744}</t>
+          <t>{2ECE1F1B-C143-4CE2-B550-348BEE185974}</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>486</v>
+        <v>413</v>
       </c>
       <c r="D27" t="n">
-        <v>499</v>
+        <v>429</v>
       </c>
       <c r="E27" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" t="inlineStr">
         <is>
-          <t>تماجيد نهضة العذراء</t>
+          <t>مقدمة الذوكصولوجيات</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{7DE226B6-2157-492D-AB80-4448CDB8A41A}</t>
+          <t>{D72E4090-F25E-47FA-91CC-49FA1BFA5556}</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>500</v>
+        <v>430</v>
       </c>
       <c r="D28" t="n">
-        <v>500</v>
+        <v>442</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" ht="18.75" customHeight="1">
       <c r="A29" t="inlineStr">
         <is>
-          <t>لحن شيري ماريا</t>
+          <t>الذكصولوجيات</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{1E7E7987-2CAA-4858-AB80-5A0AF761B6EF}</t>
+          <t>{A5B9CE2F-90E3-44D7-B22F-CAE6783C8E2F}</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>501</v>
+        <v>443</v>
       </c>
       <c r="D29" t="n">
-        <v>520</v>
+        <v>443</v>
       </c>
       <c r="E29" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" t="inlineStr">
         <is>
-          <t>إك اسماروؤت</t>
+          <t>مقدمة قانون الإيمان</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{D2101135-3E00-460B-BDBC-0ED4AE799C01}</t>
+          <t>{409B3D0A-B40A-4475-811D-72C5125134AB}</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>521</v>
+        <v>444</v>
       </c>
       <c r="D30" t="n">
-        <v>521</v>
+        <v>446</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" ht="18.75" customHeight="1">
       <c r="A31" t="inlineStr">
         <is>
-          <t>لحن شيرى ثيؤطوكى</t>
+          <t>قانون الايمان</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{18389A37-F3FC-4832-AAAE-BB56BAA2569D}</t>
+          <t>{3CD34DC9-72C7-4E1F-A24E-3878EF0435D6}</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>522</v>
+        <v>447</v>
       </c>
       <c r="D31" t="n">
-        <v>528</v>
+        <v>450</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>لحن أو كيريوس</t>
+          <t>افنوتي ناي نان</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>{9374086D-AF79-49C7-AD9E-A4DD1D98361A}</t>
+          <t>{61880C5D-7B19-4DA9-9517-587F0006E7A4}</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>529</v>
+        <v>451</v>
       </c>
       <c r="D32" t="n">
-        <v>543</v>
+        <v>459</v>
       </c>
       <c r="E32" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>شاشف إنسوب إمميني</t>
+          <t>ايطاف اني اسخاي</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{93BD22E8-BF7D-4E60-A57A-13DAE76001A3}</t>
+          <t>{60A6EF5E-A7D1-4E39-AAE6-A0EA92726711}</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>544</v>
+        <v>460</v>
       </c>
       <c r="D33" t="n">
-        <v>581</v>
+        <v>473</v>
       </c>
       <c r="E33" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" ht="18.75" customHeight="1">
       <c r="A34" t="inlineStr">
         <is>
-          <t>لحن راشى نى</t>
+          <t>طرح عيد الصليب</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{0506AF9A-7F49-49A6-942D-C2D14565C280}</t>
+          <t>{17F6A454-5ABF-4DFB-A78A-D146D086082D}</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>582</v>
+        <v>474</v>
       </c>
       <c r="D34" t="n">
-        <v>596</v>
+        <v>478</v>
       </c>
       <c r="E34" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ذفتية بانديس</t>
+          <t>طرح اخر لعيد الصليب</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>{E63D9888-2FCA-494A-AA68-15E76387F435}</t>
+          <t>{0BD005D7-2E83-417A-9686-5430EAAF391B}</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>597</v>
+        <v>479</v>
       </c>
       <c r="D35" t="n">
-        <v>621</v>
+        <v>483</v>
       </c>
       <c r="E35" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" ht="18.75" customHeight="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>سينا اتشو</t>
+          <t>مرد طرح عيد الصليب</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{63C8AA8A-342F-4B05-BFCE-A3098B55F558}</t>
+          <t>{68F134B0-811C-48F0-A7D0-5BB19CE61443}</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>622</v>
+        <v>484</v>
       </c>
       <c r="D36" t="n">
-        <v>633</v>
+        <v>484</v>
       </c>
       <c r="E36" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>فاي بى إبليمين</t>
+          <t>أفرحى يا مريم</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{01E8A009-C53E-4034-AA0C-E39290F9C47E}</t>
+          <t>{1C20AEEF-0DEB-4F74-A46A-AFC5A06DC744}</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>634</v>
+        <v>485</v>
       </c>
       <c r="D37" t="n">
-        <v>650</v>
+        <v>498</v>
       </c>
       <c r="E37" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>اطاي بارثينوس</t>
+          <t>تماجيد نهضة العذراء</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>{18835C90-087E-4BAC-9D66-708BC1E04983}</t>
+          <t>{7DE226B6-2157-492D-AB80-4448CDB8A41A}</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>651</v>
+        <v>499</v>
       </c>
       <c r="D38" t="n">
-        <v>672</v>
+        <v>499</v>
       </c>
       <c r="E38" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" ht="18.75" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>او اون او هلبيس</t>
+          <t>لحن شيري ماريا</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>{1F005296-1C13-4026-A9B3-26C9C6CD6D9D}</t>
+          <t>{1E7E7987-2CAA-4858-AB80-5A0AF761B6EF}</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>673</v>
+        <v>500</v>
       </c>
       <c r="D39" t="n">
-        <v>677</v>
+        <v>519</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" ht="18.75" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>اري ابريسفافين</t>
+          <t>إك اسماروؤت</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{08694BF7-6D62-4C4C-BA7C-6CFED091D44A}</t>
+          <t>{D2101135-3E00-460B-BDBC-0ED4AE799C01}</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>678</v>
+        <v>520</v>
       </c>
       <c r="D40" t="n">
-        <v>679</v>
+        <v>520</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ابؤرو</t>
+          <t>لحن شيرى ثيؤطوكى</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>{DD757736-F2EB-40FA-9016-1E28087A0BE5}</t>
+          <t>{18389A37-F3FC-4832-AAAE-BB56BAA2569D}</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>680</v>
+        <v>521</v>
       </c>
       <c r="D41" t="n">
-        <v>684</v>
+        <v>527</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" ht="18.75" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>مديح السلام لك يا مريم</t>
+          <t>لحن أو كيريوس</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>{1796645F-35B4-4F6F-9673-838DE7EF8F58}</t>
+          <t>{9374086D-AF79-49C7-AD9E-A4DD1D98361A}</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>685</v>
+        <v>528</v>
       </c>
       <c r="D42" t="n">
-        <v>715</v>
+        <v>542</v>
       </c>
       <c r="E42" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" ht="18.75" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>خين أفران</t>
+          <t>شاشف إنسوب إمميني</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{FD75781B-0996-4E12-BF4C-D163B4D1708F}</t>
+          <t>{93BD22E8-BF7D-4E60-A57A-13DAE76001A3}</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>716</v>
+        <v>543</v>
       </c>
       <c r="D43" t="n">
-        <v>718</v>
+        <v>580</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>اسمعي يا ابنة</t>
+          <t>لحن راشى نى</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{3C5D9889-94E1-4B35-82B5-58786720BA8A}</t>
+          <t>{0506AF9A-7F49-49A6-942D-C2D14565C280}</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>719</v>
+        <v>581</v>
       </c>
       <c r="D44" t="n">
-        <v>723</v>
+        <v>595</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>اوشية الانجيل</t>
+          <t>ذفتية بانديس</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{B897D380-076C-414A-9934-423AA6230FED}</t>
+          <t>{E63D9888-2FCA-494A-AA68-15E76387F435}</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>724</v>
+        <v>596</v>
       </c>
       <c r="D45" t="n">
-        <v>745</v>
+        <v>620</v>
       </c>
       <c r="E45" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" ht="18.75" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>طواف مزمور عيد النيروز</t>
+          <t>سينا اتشو</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{A05C62FF-6D7E-4E98-A99D-9A598F41AECB}</t>
+          <t>{63C8AA8A-342F-4B05-BFCE-A3098B55F558}</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>746</v>
+        <v>621</v>
       </c>
       <c r="D46" t="n">
-        <v>747</v>
+        <v>632</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>مرد مزمور النيروز</t>
+          <t>فاي بى إبليمين</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{11818F8A-85CC-4811-BF72-D444EBE28DB4}</t>
+          <t>{01E8A009-C53E-4034-AA0C-E39290F9C47E}</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>748</v>
+        <v>633</v>
       </c>
       <c r="D47" t="n">
-        <v>749</v>
+        <v>649</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>طواف مزمور عيد الصليب و أحد الشعانين</t>
+          <t>اطاي بارثينوس</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{FD80A82A-8C5C-4D6C-9644-19E9CC3FEC0F}</t>
+          <t>{18835C90-087E-4BAC-9D66-708BC1E04983}</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="D48" t="n">
-        <v>751</v>
+        <v>671</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" ht="18.75" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>مرد مزمور الصليب</t>
+          <t>او اون او هلبيس</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{0BC1F8D8-BE35-4C07-A134-EAB9CF63D177}</t>
+          <t>{1F005296-1C13-4026-A9B3-26C9C6CD6D9D}</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>752</v>
+        <v>672</v>
       </c>
       <c r="D49" t="n">
-        <v>753</v>
+        <v>676</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>مرد مزمور الشعانين</t>
+          <t>اري ابريسفافين</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{2AA95ED2-79CB-40D2-B716-1CB9E9E65C87}</t>
+          <t>{08694BF7-6D62-4C4C-BA7C-6CFED091D44A}</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>754</v>
+        <v>677</v>
       </c>
       <c r="D50" t="n">
-        <v>754</v>
+        <v>678</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" ht="18.75" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>مزمور صوم وعشيات اعياد السيدة العذراء</t>
+          <t>ابؤرو</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{AB54231C-F141-461A-8580-187ADC04F4DB}</t>
+          <t>{DD757736-F2EB-40FA-9016-1E28087A0BE5}</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>755</v>
+        <v>679</v>
       </c>
       <c r="D51" t="n">
-        <v>757</v>
+        <v>683</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" ht="18.75" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>طواف صوم واعياد العذراء</t>
+          <t>مديح السلام لك يا مريم</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>{AD767EA5-20E9-48D6-9567-43335CC42D9A}</t>
+          <t>{1796645F-35B4-4F6F-9673-838DE7EF8F58}</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>758</v>
+        <v>684</v>
       </c>
       <c r="D52" t="n">
-        <v>760</v>
+        <v>714</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" ht="18.75" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>مارو اتشاسف</t>
+          <t>خين أفران</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>{62A12AF8-CB6D-4CC5-9DB0-B73A7C24E2AD}</t>
+          <t>{FD75781B-0996-4E12-BF4C-D163B4D1708F}</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>761</v>
+        <v>715</v>
       </c>
       <c r="D53" t="n">
-        <v>770</v>
+        <v>717</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
       <c r="A54" t="inlineStr">
         <is>
-          <t>مقدمة الانجيل</t>
+          <t>اسمعي يا ابنة</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>{C9DDD86A-610C-49CA-81D2-F3293213F325}</t>
+          <t>{3C5D9889-94E1-4B35-82B5-58786720BA8A}</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="D54" t="n">
-        <v>780</v>
+        <v>722</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" ht="18.75" customHeight="1">
       <c r="A55" t="inlineStr">
         <is>
-          <t>الانجيل قبطي</t>
+          <t>اوشية الانجيل</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>{B900AA98-6A60-4787-8E81-4111C4CE8DC1}</t>
+          <t>{B897D380-076C-414A-9934-423AA6230FED}</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>781</v>
+        <v>723</v>
       </c>
       <c r="D55" t="n">
-        <v>784</v>
+        <v>744</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" ht="18.75" customHeight="1">
       <c r="A56" t="inlineStr">
         <is>
-          <t>الانجيل</t>
+          <t>طواف مزمور عيد النيروز</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>{B74DBB8C-2B2D-46E4-9508-DA46008D19A4}</t>
+          <t>{A05C62FF-6D7E-4E98-A99D-9A598F41AECB}</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>785</v>
+        <v>745</v>
       </c>
       <c r="D56" t="n">
-        <v>791</v>
+        <v>746</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" ht="18.75" customHeight="1">
       <c r="A57" t="inlineStr">
         <is>
-          <t>مرد انجيل الصليب</t>
+          <t>مرد مزمور النيروز</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>{EDE09087-B069-49CA-8211-757926594D3F}</t>
+          <t>{11818F8A-85CC-4811-BF72-D444EBE28DB4}</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>792</v>
+        <v>747</v>
       </c>
       <c r="D57" t="n">
-        <v>794</v>
+        <v>748</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" ht="18.75" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>مرد انجيل عشية الشعانين</t>
+          <t>طواف مزمور عيد الصليب و أحد الشعانين</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>{995B3A40-EED6-4463-A2DC-498DF1965406}</t>
+          <t>{FD80A82A-8C5C-4D6C-9644-19E9CC3FEC0F}</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>795</v>
+        <v>749</v>
       </c>
       <c r="D58" t="n">
-        <v>796</v>
+        <v>750</v>
       </c>
       <c r="E58" t="n">
         <v>2</v>
@@ -22445,40 +22442,40 @@
     <row r="59" ht="18.75" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>مرد انجيل باكر الشعانين</t>
+          <t>مرد مزمور الصليب</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>{AE580C60-FE10-48A4-8A58-816566E88A65}</t>
+          <t>{0BC1F8D8-BE35-4C07-A134-EAB9CF63D177}</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>797</v>
+        <v>751</v>
       </c>
       <c r="D59" t="n">
-        <v>799</v>
+        <v>752</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" ht="18.75" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
-          <t>مرد انجيل التجلي</t>
+          <t>مرد مزمور الشعانين</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>{424645C4-4007-414C-8960-3DE1095D0419}</t>
+          <t>{2AA95ED2-79CB-40D2-B716-1CB9E9E65C87}</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>800</v>
+        <v>753</v>
       </c>
       <c r="D60" t="n">
-        <v>800</v>
+        <v>753</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
@@ -22487,124 +22484,124 @@
     <row r="61" ht="18.75" customHeight="1">
       <c r="A61" t="inlineStr">
         <is>
-          <t>فاي اريه بي اوو</t>
+          <t>مزمور صوم وعشيات اعياد السيدة العذراء</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>{B7D98377-B994-4654-B49C-DE10E0DDE4F1}</t>
+          <t>{AB54231C-F141-461A-8580-187ADC04F4DB}</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>801</v>
+        <v>754</v>
       </c>
       <c r="D61" t="n">
-        <v>801</v>
+        <v>756</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" ht="18.75" customHeight="1">
       <c r="A62" t="inlineStr">
         <is>
-          <t>مرد الانجيل السنوي</t>
+          <t>طواف صوم واعياد العذراء</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>{BEECCC68-2AEF-4568-91AA-98BCD14D3B92}</t>
+          <t>{AD767EA5-20E9-48D6-9567-43335CC42D9A}</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>802</v>
+        <v>757</v>
       </c>
       <c r="D62" t="n">
-        <v>803</v>
+        <v>759</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" ht="18.75" customHeight="1">
       <c r="A63" t="inlineStr">
         <is>
-          <t>مرد انجيل كيهك 1</t>
+          <t>مارو اتشاسف</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>{765066DC-37D0-48B3-9046-D4F98F5B05BC}</t>
+          <t>{62A12AF8-CB6D-4CC5-9DB0-B73A7C24E2AD}</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>804</v>
+        <v>760</v>
       </c>
       <c r="D63" t="n">
-        <v>805</v>
+        <v>769</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" ht="18.75" customHeight="1">
       <c r="A64" t="inlineStr">
         <is>
-          <t>مرد انجيل كيهك 2</t>
+          <t>مقدمة الانجيل</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>{D5E69BAC-0157-4B69-9255-B6775E2EE11D}</t>
+          <t>{C9DDD86A-610C-49CA-81D2-F3293213F325}</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>806</v>
+        <v>770</v>
       </c>
       <c r="D64" t="n">
-        <v>807</v>
+        <v>779</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" ht="18.75" customHeight="1">
       <c r="A65" t="inlineStr">
         <is>
-          <t>تكملة مشتركة لكيهك</t>
+          <t>الانجيل قبطي</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>{98BAFA87-CFC9-4304-8B00-99AA9EC72A3D}</t>
+          <t>{B900AA98-6A60-4787-8E81-4111C4CE8DC1}</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>808</v>
+        <v>780</v>
       </c>
       <c r="D65" t="n">
-        <v>809</v>
+        <v>783</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" ht="18.75" customHeight="1">
       <c r="A66" t="inlineStr">
         <is>
-          <t>مرد انجيل صوم العذراء - عشية</t>
+          <t>المزمور</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>{5043F523-486A-4B7C-9F73-2F3F943BB30C}</t>
+          <t>{6D1E6E7D-EECE-483C-A3AE-C135D02E717C}</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>810</v>
+        <v>784</v>
       </c>
       <c r="D66" t="n">
-        <v>811</v>
+        <v>785</v>
       </c>
       <c r="E66" t="n">
         <v>2</v>
@@ -22613,40 +22610,40 @@
     <row r="67" ht="18.75" customHeight="1">
       <c r="A67" t="inlineStr">
         <is>
-          <t>مرد انجيل صوم العذراء - باكر</t>
+          <t>فليرفعوه</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>{037D8578-7219-4388-AFC5-4753352BFA8C}</t>
+          <t>{23533FC3-43FE-456F-9454-70C3088055E7}</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>812</v>
+        <v>786</v>
       </c>
       <c r="D67" t="n">
-        <v>812</v>
+        <v>788</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" ht="18.75" customHeight="1">
       <c r="A68" t="inlineStr">
         <is>
-          <t>اري ابرسفافين</t>
+          <t>الانجيل</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>{49534D46-CF48-4D9B-ADBF-B776827F6670}</t>
+          <t>{B74DBB8C-2B2D-46E4-9508-DA46008D19A4}</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>813</v>
+        <v>789</v>
       </c>
       <c r="D68" t="n">
-        <v>814</v>
+        <v>790</v>
       </c>
       <c r="E68" t="n">
         <v>2</v>
@@ -22655,40 +22652,40 @@
     <row r="69" ht="18.75" customHeight="1">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ربع يقال في صوم الرسل</t>
+          <t>مرد انجيل الصليب</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>{F5AB11D4-D7D2-4DA3-A830-32BA45BCB16D}</t>
+          <t>{EDE09087-B069-49CA-8211-757926594D3F}</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>815</v>
+        <v>791</v>
       </c>
       <c r="D69" t="n">
-        <v>816</v>
+        <v>793</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="18.75" customHeight="1">
       <c r="A70" t="inlineStr">
         <is>
-          <t>جي افسمارؤوت</t>
+          <t>مرد انجيل عشية الشعانين</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>{DD53DBD3-9599-4D1D-B8C1-EAB35FBD36D3}</t>
+          <t>{995B3A40-EED6-4463-A2DC-498DF1965406}</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>817</v>
+        <v>794</v>
       </c>
       <c r="D70" t="n">
-        <v>818</v>
+        <v>795</v>
       </c>
       <c r="E70" t="n">
         <v>2</v>
@@ -22697,277 +22694,528 @@
     <row r="71" ht="18.75" customHeight="1">
       <c r="A71" t="inlineStr">
         <is>
-          <t>اوشية السلام</t>
+          <t>مرد انجيل باكر الشعانين</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>{4DB48091-D529-44E1-939A-81BC51E41D41}</t>
+          <t>{AE580C60-FE10-48A4-8A58-816566E88A65}</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>819</v>
+        <v>796</v>
       </c>
       <c r="D71" t="n">
-        <v>831</v>
+        <v>798</v>
       </c>
       <c r="E71" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" ht="18.75" customHeight="1">
       <c r="A72" t="inlineStr">
         <is>
-          <t>اوشية الآباء</t>
+          <t>مرد انجيل التجلي</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>{64C3B268-ED69-4006-B650-A09460633196}</t>
+          <t>{424645C4-4007-414C-8960-3DE1095D0419}</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>832</v>
+        <v>799</v>
       </c>
       <c r="D72" t="n">
-        <v>840</v>
+        <v>799</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" ht="18.75" customHeight="1">
       <c r="A73" t="inlineStr">
         <is>
-          <t>أوشية الموضع</t>
+          <t>فاي اريه بي اوو</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>{9DACDA4B-74BF-4F4B-A961-DA43C70DC545}</t>
+          <t>{B7D98377-B994-4654-B49C-DE10E0DDE4F1}</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>841</v>
+        <v>800</v>
       </c>
       <c r="D73" t="n">
-        <v>849</v>
+        <v>800</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" ht="18.75" customHeight="1">
       <c r="A74" t="inlineStr">
         <is>
-          <t>تكملة الاواشي</t>
+          <t>مرد الانجيل السنوي</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>{5DFBA264-6756-41DD-8F16-17B76F3E3F0F}</t>
+          <t>{BEECCC68-2AEF-4568-91AA-98BCD14D3B92}</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>850</v>
+        <v>801</v>
       </c>
       <c r="D74" t="n">
-        <v>864</v>
+        <v>802</v>
       </c>
       <c r="E74" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" ht="18.75" customHeight="1">
       <c r="A75" t="inlineStr">
         <is>
-          <t>أوشية الإجتماعات</t>
+          <t>مرد انجيل كيهك 1</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>{7259AEAC-8F21-4B0E-9C69-498513DD91E4}</t>
+          <t>{765066DC-37D0-48B3-9046-D4F98F5B05BC}</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>865</v>
+        <v>803</v>
       </c>
       <c r="D75" t="n">
-        <v>890</v>
+        <v>804</v>
       </c>
       <c r="E75" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" ht="18.75" customHeight="1">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ابانا الذي في السموات</t>
+          <t>مرد انجيل كيهك 2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>{FD187B58-5CE8-4776-8487-9C5928B14F0D}</t>
+          <t>{D5E69BAC-0157-4B69-9255-B6775E2EE11D}</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>891</v>
+        <v>805</v>
       </c>
       <c r="D76" t="n">
-        <v>897</v>
+        <v>806</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" ht="18.75" customHeight="1">
       <c r="A77" t="inlineStr">
         <is>
-          <t>الختام</t>
+          <t>تكملة مشتركة لكيهك</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>{90F50AB7-3911-445D-9C45-41866ECCCED0}</t>
+          <t>{98BAFA87-CFC9-4304-8B00-99AA9EC72A3D}</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>898</v>
+        <v>807</v>
       </c>
       <c r="D77" t="n">
-        <v>900</v>
+        <v>808</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" ht="18.75" customHeight="1">
       <c r="A78" t="inlineStr">
         <is>
-          <t>تكملة على حسب المناسبة</t>
+          <t>مرد انجيل صوم العذراء - عشية</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>{A18EDC94-F257-4FAC-99C7-0A8EA70F0FAF}</t>
+          <t>{5043F523-486A-4B7C-9F73-2F3F943BB30C}</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>901</v>
+        <v>809</v>
       </c>
       <c r="D78" t="n">
-        <v>919</v>
+        <v>810</v>
       </c>
       <c r="E78" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" ht="18.75" customHeight="1">
       <c r="A79" t="inlineStr">
         <is>
-          <t>في حضور الاسقف</t>
+          <t>مرد انجيل صوم العذراء - باكر</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>{A9183893-7B7E-459F-8547-F7A8F7D2D521}</t>
+          <t>{037D8578-7219-4388-AFC5-4753352BFA8C}</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>920</v>
+        <v>811</v>
       </c>
       <c r="D79" t="n">
-        <v>928</v>
+        <v>811</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" ht="18.75" customHeight="1">
       <c r="A80" t="inlineStr">
         <is>
-          <t>الختام 2</t>
+          <t>اري ابرسفافين</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>{A3DED752-5159-4F64-86F6-7B95F37A8327}</t>
+          <t>{49534D46-CF48-4D9B-ADBF-B776827F6670}</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>929</v>
+        <v>812</v>
       </c>
       <c r="D80" t="n">
-        <v>933</v>
+        <v>813</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" ht="18.75" customHeight="1">
       <c r="A81" t="inlineStr">
         <is>
-          <t>اوشية المياة</t>
+          <t>ربع يقال في صوم الرسل</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>{BA51DE45-1C6C-43E6-AFF3-A98C3B049C70}</t>
+          <t>{F5AB11D4-D7D2-4DA3-A830-32BA45BCB16D}</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>934</v>
+        <v>814</v>
       </c>
       <c r="D81" t="n">
-        <v>940</v>
+        <v>815</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" ht="18.75" customHeight="1">
       <c r="A82" t="inlineStr">
         <is>
-          <t>أوشية الزروع</t>
+          <t>جي افسمارؤوت</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>{A0DD24B6-1053-42A1-8391-038649B3219B}</t>
+          <t>{DD53DBD3-9599-4D1D-B8C1-EAB35FBD36D3}</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>941</v>
+        <v>816</v>
       </c>
       <c r="D82" t="n">
-        <v>948</v>
+        <v>817</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" ht="18.75" customHeight="1">
       <c r="A83" t="inlineStr">
         <is>
+          <t>اوشية السلام</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>{4DB48091-D529-44E1-939A-81BC51E41D41}</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>818</v>
+      </c>
+      <c r="D83" t="n">
+        <v>830</v>
+      </c>
+      <c r="E83" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" ht="18.75" customHeight="1">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>اوشية الآباء</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>{64C3B268-ED69-4006-B650-A09460633196}</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>831</v>
+      </c>
+      <c r="D84" t="n">
+        <v>839</v>
+      </c>
+      <c r="E84" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" ht="18.75" customHeight="1">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>أوشية الموضع</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>{9DACDA4B-74BF-4F4B-A961-DA43C70DC545}</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>840</v>
+      </c>
+      <c r="D85" t="n">
+        <v>848</v>
+      </c>
+      <c r="E85" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" ht="18.75" customHeight="1">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>تكملة الاواشي</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>{5DFBA264-6756-41DD-8F16-17B76F3E3F0F}</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>849</v>
+      </c>
+      <c r="D86" t="n">
+        <v>863</v>
+      </c>
+      <c r="E86" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" ht="18.75" customHeight="1">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>أوشية الإجتماعات</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>{7259AEAC-8F21-4B0E-9C69-498513DD91E4}</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>864</v>
+      </c>
+      <c r="D87" t="n">
+        <v>889</v>
+      </c>
+      <c r="E87" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" ht="18.75" customHeight="1">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ابانا الذي في السموات</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>{FD187B58-5CE8-4776-8487-9C5928B14F0D}</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>890</v>
+      </c>
+      <c r="D88" t="n">
+        <v>896</v>
+      </c>
+      <c r="E88" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" ht="18.75" customHeight="1">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>الختام</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>{90F50AB7-3911-445D-9C45-41866ECCCED0}</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>897</v>
+      </c>
+      <c r="D89" t="n">
+        <v>899</v>
+      </c>
+      <c r="E89" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" ht="18.75" customHeight="1">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>تكملة على حسب المناسبة</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>{A18EDC94-F257-4FAC-99C7-0A8EA70F0FAF}</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>900</v>
+      </c>
+      <c r="D90" t="n">
+        <v>918</v>
+      </c>
+      <c r="E90" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" ht="18.75" customHeight="1">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>في حضور الاسقف</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>{A9183893-7B7E-459F-8547-F7A8F7D2D521}</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>919</v>
+      </c>
+      <c r="D91" t="n">
+        <v>927</v>
+      </c>
+      <c r="E91" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" ht="18.75" customHeight="1">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>الختام 2</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>{A3DED752-5159-4F64-86F6-7B95F37A8327}</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>928</v>
+      </c>
+      <c r="D92" t="n">
+        <v>932</v>
+      </c>
+      <c r="E92" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" ht="18.75" customHeight="1">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>اوشية المياة</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>{BA51DE45-1C6C-43E6-AFF3-A98C3B049C70}</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>933</v>
+      </c>
+      <c r="D93" t="n">
+        <v>939</v>
+      </c>
+      <c r="E93" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" ht="18.75" customHeight="1">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>أوشية الزروع</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>{A0DD24B6-1053-42A1-8391-038649B3219B}</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>940</v>
+      </c>
+      <c r="D94" t="n">
+        <v>947</v>
+      </c>
+      <c r="E94" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" ht="18.75" customHeight="1">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>اوشية الأهوية والثمار</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>{BD1D9BBC-5109-4880-BAFF-4C03F37555C1}</t>
         </is>
       </c>
-      <c r="C83" t="n">
-        <v>949</v>
-      </c>
-      <c r="D83" t="n">
-        <v>954</v>
-      </c>
-      <c r="E83" t="n">
+      <c r="C95" t="n">
+        <v>948</v>
+      </c>
+      <c r="D95" t="n">
+        <v>953</v>
+      </c>
+      <c r="E95" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="84" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22989,9 +23237,9 @@
   <cols>
     <col width="19.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -23945,9 +24193,9 @@
   <cols>
     <col width="17.005" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -24146,9 +24394,9 @@
   <cols>
     <col width="21.005" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -25543,7 +25791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" ht="18.75" customHeight="1">
       <c r="A67" t="inlineStr">
         <is>
           <t>قدوس قدوس قدوس</t>
@@ -25585,9 +25833,9 @@
   <cols>
     <col width="28.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="16.43357142857143" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="16.43357142857143" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">

</xml_diff>